<commit_message>
Updated Organizer with New file structure
</commit_message>
<xml_diff>
--- a/src/Input_Files/cultures.xlsx
+++ b/src/Input_Files/cultures.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python Scripts\imperator\ProvinceOrganizer\EP_ImperatorProvinceOrganizer\src\Input_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B7CDB07-D772-46A5-B1C4-1B32A6862D3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FCF349C-316B-4161-A92B-938BC365C29B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10500" yWindow="2490" windowWidth="21600" windowHeight="10800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1215" yWindow="1515" windowWidth="21600" windowHeight="10800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Culture</t>
   </si>
@@ -127,6 +127,36 @@
   </si>
   <si>
     <t>Hiberno-Norman</t>
+  </si>
+  <si>
+    <t>arpitan</t>
+  </si>
+  <si>
+    <t>(81, 114, 255)</t>
+  </si>
+  <si>
+    <t>basque</t>
+  </si>
+  <si>
+    <t>(41, 146, 17)</t>
+  </si>
+  <si>
+    <t>walloon</t>
+  </si>
+  <si>
+    <t>(131, 127, 37)</t>
+  </si>
+  <si>
+    <t>picard</t>
+  </si>
+  <si>
+    <t>(110, 120, 161)</t>
+  </si>
+  <si>
+    <t>norman</t>
+  </si>
+  <si>
+    <t>(243, 13, 13)</t>
   </si>
 </sst>
 </file>
@@ -449,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,6 +627,46 @@
         <v>25</v>
       </c>
     </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>